<commit_message>
change style navbar enseignant
</commit_message>
<xml_diff>
--- a/projet/wwwroot/FichierAddDBEnseignants/addlistmodules.xlsx
+++ b/projet/wwwroot/FichierAddDBEnseignants/addlistmodules.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\plus_ ma_part\projet-dotnet-core-master\projet\wwwroot\FichierAddDBEnseignants\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\s8\Version git\projet-dotnet-core\projet\wwwroot\FichierAddDBEnseignants\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FEB745-D740-4AC5-9755-0C55C3B2C6D5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2115" yWindow="2115" windowWidth="15375" windowHeight="7875" xr2:uid="{248D2CB0-A935-4225-AF7A-D976AA54D653}"/>
+    <workbookView xWindow="2112" yWindow="2112" windowWidth="15372" windowHeight="7872"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -59,7 +58,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -404,16 +403,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA58C48-0720-42B3-B9AA-557765543630}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -421,7 +420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -429,7 +428,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -437,7 +436,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -445,7 +444,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>

</xml_diff>